<commit_message>
Updated ReadData.py to include all data files and convert valence/arousal to engagement
</commit_message>
<xml_diff>
--- a/Excel/4.xlsx
+++ b/Excel/4.xlsx
@@ -1,26 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26207"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maryprouty/Desktop/MUC-Project/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gopal\Documents\School\Classes\Graduate_Classes\UbiquitousComputing\MUC-Project\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988F9F72-6CC9-4810-9493-A85D10D9753E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="460" windowWidth="16000" windowHeight="16000"/>
+    <workbookView xWindow="16500" yWindow="225" windowWidth="10770" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -28,21 +35,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="26">
-  <si>
-    <t>seconds</t>
-  </si>
-  <si>
-    <t>class activity</t>
-  </si>
-  <si>
-    <t>specific behavior</t>
-  </si>
-  <si>
-    <t>valence</t>
-  </si>
-  <si>
-    <t>arousal</t>
-  </si>
   <si>
     <t>drawing example</t>
   </si>
@@ -106,11 +98,26 @@
   <si>
     <t>Nodding</t>
   </si>
+  <si>
+    <t>Seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Class Activity </t>
+  </si>
+  <si>
+    <t>Specific Behvaior</t>
+  </si>
+  <si>
+    <t>Valence</t>
+  </si>
+  <si>
+    <t>Arousal</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -455,49 +462,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="C222" sqref="C222"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.83203125" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="7" max="7" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -506,18 +513,18 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -526,18 +533,18 @@
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -546,19 +553,19 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>A4 + 10</f>
         <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -567,16 +574,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>A5 + 10</f>
         <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -585,16 +592,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ref="A7:A70" si="0">A6 + 10</f>
         <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D7">
         <v>3</v>
@@ -603,16 +610,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -621,16 +628,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -639,16 +646,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -657,16 +664,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -675,16 +682,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -693,16 +700,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -711,16 +718,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -729,16 +736,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>130</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D15">
         <v>3</v>
@@ -747,16 +754,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>140</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D16">
         <v>3</v>
@@ -765,16 +772,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D17">
         <v>3</v>
@@ -783,16 +790,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>160</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -801,16 +808,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>170</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -819,16 +826,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -837,16 +844,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D21">
         <v>3</v>
@@ -855,16 +862,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D22">
         <v>3</v>
@@ -873,16 +880,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>210</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D23">
         <v>3</v>
@@ -891,16 +898,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>220</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D24">
         <v>3</v>
@@ -909,16 +916,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>230</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D25">
         <v>4</v>
@@ -927,16 +934,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D26">
         <v>3</v>
@@ -945,16 +952,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D27">
         <v>3</v>
@@ -963,16 +970,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>260</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D28">
         <v>2</v>
@@ -981,16 +988,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>270</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D29">
         <v>3</v>
@@ -999,16 +1006,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>280</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D30">
         <v>3</v>
@@ -1017,16 +1024,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>290</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D31">
         <v>3</v>
@@ -1035,16 +1042,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -1053,16 +1060,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>310</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D33">
         <v>3</v>
@@ -1071,16 +1078,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>320</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D34">
         <v>3</v>
@@ -1089,16 +1096,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>330</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D35">
         <v>3</v>
@@ -1107,16 +1114,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>340</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D36">
         <v>3</v>
@@ -1125,16 +1132,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>350</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D37">
         <v>3</v>
@@ -1143,16 +1150,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>360</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D38">
         <v>3</v>
@@ -1161,16 +1168,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>370</v>
       </c>
       <c r="B39" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D39">
         <v>3</v>
@@ -1179,16 +1186,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>380</v>
       </c>
       <c r="B40" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D40">
         <v>4</v>
@@ -1197,250 +1204,250 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>390</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41">
+        <v>3</v>
+      </c>
+      <c r="E41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42">
+        <v>3</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>410</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>420</v>
+      </c>
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44">
+        <v>3</v>
+      </c>
+      <c r="E44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>430</v>
+      </c>
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+      <c r="E45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>440</v>
+      </c>
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46">
+        <v>3</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>450</v>
+      </c>
+      <c r="B47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47">
+        <v>3</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" si="0"/>
+        <v>460</v>
+      </c>
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+      <c r="E48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>470</v>
+      </c>
+      <c r="B49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49">
+        <v>3</v>
+      </c>
+      <c r="E49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" si="0"/>
+        <v>480</v>
+      </c>
+      <c r="B50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" si="0"/>
+        <v>490</v>
+      </c>
+      <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51">
+        <v>3</v>
+      </c>
+      <c r="E51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52">
+        <v>3</v>
+      </c>
+      <c r="E52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f t="shared" si="0"/>
+        <v>510</v>
+      </c>
+      <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53">
+        <v>3</v>
+      </c>
+      <c r="E53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f t="shared" si="0"/>
+        <v>520</v>
+      </c>
+      <c r="B54" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" t="s">
         <v>15</v>
-      </c>
-      <c r="D41">
-        <v>3</v>
-      </c>
-      <c r="E41">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <f t="shared" si="0"/>
-        <v>400</v>
-      </c>
-      <c r="B42" t="s">
-        <v>10</v>
-      </c>
-      <c r="C42" t="s">
-        <v>15</v>
-      </c>
-      <c r="D42">
-        <v>3</v>
-      </c>
-      <c r="E42">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <f t="shared" si="0"/>
-        <v>410</v>
-      </c>
-      <c r="B43" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" t="s">
-        <v>15</v>
-      </c>
-      <c r="D43">
-        <v>3</v>
-      </c>
-      <c r="E43">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <f t="shared" si="0"/>
-        <v>420</v>
-      </c>
-      <c r="B44" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" t="s">
-        <v>15</v>
-      </c>
-      <c r="D44">
-        <v>3</v>
-      </c>
-      <c r="E44">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <f t="shared" si="0"/>
-        <v>430</v>
-      </c>
-      <c r="B45" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" t="s">
-        <v>15</v>
-      </c>
-      <c r="D45">
-        <v>3</v>
-      </c>
-      <c r="E45">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <f t="shared" si="0"/>
-        <v>440</v>
-      </c>
-      <c r="B46" t="s">
-        <v>10</v>
-      </c>
-      <c r="C46" t="s">
-        <v>15</v>
-      </c>
-      <c r="D46">
-        <v>3</v>
-      </c>
-      <c r="E46">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <f t="shared" si="0"/>
-        <v>450</v>
-      </c>
-      <c r="B47" t="s">
-        <v>10</v>
-      </c>
-      <c r="C47" t="s">
-        <v>15</v>
-      </c>
-      <c r="D47">
-        <v>3</v>
-      </c>
-      <c r="E47">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <f t="shared" si="0"/>
-        <v>460</v>
-      </c>
-      <c r="B48" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" t="s">
-        <v>15</v>
-      </c>
-      <c r="D48">
-        <v>3</v>
-      </c>
-      <c r="E48">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <f t="shared" si="0"/>
-        <v>470</v>
-      </c>
-      <c r="B49" t="s">
-        <v>10</v>
-      </c>
-      <c r="C49" t="s">
-        <v>15</v>
-      </c>
-      <c r="D49">
-        <v>3</v>
-      </c>
-      <c r="E49">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <f t="shared" si="0"/>
-        <v>480</v>
-      </c>
-      <c r="B50" t="s">
-        <v>10</v>
-      </c>
-      <c r="C50" t="s">
-        <v>15</v>
-      </c>
-      <c r="D50">
-        <v>3</v>
-      </c>
-      <c r="E50">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <f t="shared" si="0"/>
-        <v>490</v>
-      </c>
-      <c r="B51" t="s">
-        <v>10</v>
-      </c>
-      <c r="C51" t="s">
-        <v>15</v>
-      </c>
-      <c r="D51">
-        <v>3</v>
-      </c>
-      <c r="E51">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-      <c r="B52" t="s">
-        <v>10</v>
-      </c>
-      <c r="C52" t="s">
-        <v>15</v>
-      </c>
-      <c r="D52">
-        <v>3</v>
-      </c>
-      <c r="E52">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <f t="shared" si="0"/>
-        <v>510</v>
-      </c>
-      <c r="B53" t="s">
-        <v>10</v>
-      </c>
-      <c r="C53" t="s">
-        <v>15</v>
-      </c>
-      <c r="D53">
-        <v>3</v>
-      </c>
-      <c r="E53">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <f t="shared" si="0"/>
-        <v>520</v>
-      </c>
-      <c r="B54" t="s">
-        <v>10</v>
-      </c>
-      <c r="C54" t="s">
-        <v>20</v>
       </c>
       <c r="D54">
         <v>3</v>
@@ -1449,16 +1456,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>530</v>
       </c>
       <c r="B55" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D55">
         <v>3</v>
@@ -1467,16 +1474,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>540</v>
       </c>
       <c r="B56" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C56" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D56">
         <v>3</v>
@@ -1485,16 +1492,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>550</v>
       </c>
       <c r="B57" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D57">
         <v>3</v>
@@ -1503,16 +1510,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>560</v>
       </c>
       <c r="B58" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C58" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D58">
         <v>3</v>
@@ -1521,53 +1528,53 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>570</v>
       </c>
       <c r="B59" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C59" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59">
+        <v>3</v>
+      </c>
+      <c r="E59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f t="shared" si="0"/>
+        <v>580</v>
+      </c>
+      <c r="B60" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60">
+        <v>3</v>
+      </c>
+      <c r="E60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f t="shared" si="0"/>
+        <v>590</v>
+      </c>
+      <c r="B61" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
         <v>16</v>
       </c>
-      <c r="D59">
-        <v>3</v>
-      </c>
-      <c r="E59">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <f t="shared" si="0"/>
-        <v>580</v>
-      </c>
-      <c r="B60" t="s">
-        <v>10</v>
-      </c>
-      <c r="C60" t="s">
-        <v>15</v>
-      </c>
-      <c r="D60">
-        <v>3</v>
-      </c>
-      <c r="E60">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <f t="shared" si="0"/>
-        <v>590</v>
-      </c>
-      <c r="B61" t="s">
-        <v>10</v>
-      </c>
-      <c r="C61" t="s">
-        <v>21</v>
-      </c>
       <c r="D61">
         <v>3</v>
       </c>
@@ -1575,16 +1582,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>600</v>
       </c>
       <c r="B62" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D62">
         <v>3</v>
@@ -1593,16 +1600,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>610</v>
       </c>
       <c r="B63" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C63" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D63">
         <v>3</v>
@@ -1611,16 +1618,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>620</v>
       </c>
       <c r="B64" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C64" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D64">
         <v>3</v>
@@ -1629,16 +1636,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>630</v>
       </c>
       <c r="B65" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C65" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D65">
         <v>3</v>
@@ -1647,16 +1654,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>640</v>
       </c>
       <c r="B66" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C66" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D66">
         <v>3</v>
@@ -1665,16 +1672,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" si="0"/>
         <v>650</v>
       </c>
       <c r="B67" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C67" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D67">
         <v>3</v>
@@ -1683,16 +1690,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" si="0"/>
         <v>660</v>
       </c>
       <c r="B68" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C68" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D68">
         <v>3</v>
@@ -1701,16 +1708,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" si="0"/>
         <v>670</v>
       </c>
       <c r="B69" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C69" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D69">
         <v>3</v>
@@ -1719,16 +1726,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" si="0"/>
         <v>680</v>
       </c>
       <c r="B70" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C70" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D70">
         <v>3</v>
@@ -1737,16 +1744,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" ref="A71:A134" si="1">A70 + 10</f>
         <v>690</v>
       </c>
       <c r="B71" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C71" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D71">
         <v>3</v>
@@ -1755,16 +1762,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>700</v>
       </c>
       <c r="B72" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C72" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D72">
         <v>3</v>
@@ -1773,16 +1780,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>710</v>
       </c>
       <c r="B73" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C73" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D73">
         <v>3</v>
@@ -1791,16 +1798,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>720</v>
       </c>
       <c r="B74" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C74" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D74">
         <v>3</v>
@@ -1809,16 +1816,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>730</v>
       </c>
       <c r="B75" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C75" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D75">
         <v>3</v>
@@ -1827,16 +1834,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>740</v>
       </c>
       <c r="B76" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C76" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D76">
         <v>3</v>
@@ -1845,16 +1852,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>750</v>
       </c>
       <c r="B77" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C77" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D77">
         <v>3</v>
@@ -1863,16 +1870,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>760</v>
       </c>
       <c r="B78" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C78" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D78">
         <v>3</v>
@@ -1881,16 +1888,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>770</v>
       </c>
       <c r="B79" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C79" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D79">
         <v>3</v>
@@ -1899,16 +1906,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>780</v>
       </c>
       <c r="B80" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C80" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D80">
         <v>3</v>
@@ -1917,16 +1924,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>790</v>
       </c>
       <c r="B81" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C81" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D81">
         <v>3</v>
@@ -1935,16 +1942,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>800</v>
       </c>
       <c r="B82" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C82" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D82">
         <v>3</v>
@@ -1953,16 +1960,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>810</v>
       </c>
       <c r="B83" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C83" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D83">
         <v>3</v>
@@ -1971,16 +1978,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>820</v>
       </c>
       <c r="B84" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C84" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D84">
         <v>3</v>
@@ -1989,16 +1996,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>830</v>
       </c>
       <c r="B85" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C85" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D85">
         <v>3</v>
@@ -2007,16 +2014,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>840</v>
       </c>
       <c r="B86" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C86" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D86">
         <v>3</v>
@@ -2025,16 +2032,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>850</v>
       </c>
       <c r="B87" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C87" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D87">
         <v>3</v>
@@ -2043,16 +2050,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>860</v>
       </c>
       <c r="B88" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C88" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D88">
         <v>3</v>
@@ -2061,16 +2068,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>870</v>
       </c>
       <c r="B89" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C89" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D89">
         <v>3</v>
@@ -2079,16 +2086,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>880</v>
       </c>
       <c r="B90" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C90" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D90">
         <v>3</v>
@@ -2097,16 +2104,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>890</v>
       </c>
       <c r="B91" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C91" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D91">
         <v>3</v>
@@ -2115,16 +2122,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>900</v>
       </c>
       <c r="B92" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C92" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D92">
         <v>3</v>
@@ -2133,16 +2140,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>910</v>
       </c>
       <c r="B93" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C93" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D93">
         <v>3</v>
@@ -2151,16 +2158,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>920</v>
       </c>
       <c r="B94" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C94" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D94">
         <v>3</v>
@@ -2169,16 +2176,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>930</v>
       </c>
       <c r="B95" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C95" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D95">
         <v>3</v>
@@ -2187,16 +2194,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>940</v>
       </c>
       <c r="B96" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C96" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D96">
         <v>3</v>
@@ -2205,124 +2212,124 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>950</v>
       </c>
       <c r="B97" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C97" t="s">
+        <v>9</v>
+      </c>
+      <c r="D97">
+        <v>3</v>
+      </c>
+      <c r="E97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <f t="shared" si="1"/>
+        <v>960</v>
+      </c>
+      <c r="B98" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" t="s">
+        <v>9</v>
+      </c>
+      <c r="D98">
+        <v>3</v>
+      </c>
+      <c r="E98">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <f t="shared" si="1"/>
+        <v>970</v>
+      </c>
+      <c r="B99" t="s">
+        <v>5</v>
+      </c>
+      <c r="C99" t="s">
+        <v>9</v>
+      </c>
+      <c r="D99">
+        <v>3</v>
+      </c>
+      <c r="E99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <f t="shared" si="1"/>
+        <v>980</v>
+      </c>
+      <c r="B100" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" t="s">
+        <v>9</v>
+      </c>
+      <c r="D100">
+        <v>3</v>
+      </c>
+      <c r="E100">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <f t="shared" si="1"/>
+        <v>990</v>
+      </c>
+      <c r="B101" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" t="s">
+        <v>10</v>
+      </c>
+      <c r="D101">
+        <v>3</v>
+      </c>
+      <c r="E101">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="B102" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" t="s">
+        <v>10</v>
+      </c>
+      <c r="D102">
+        <v>3</v>
+      </c>
+      <c r="E102">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <f t="shared" si="1"/>
+        <v>1010</v>
+      </c>
+      <c r="B103" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103" t="s">
         <v>14</v>
-      </c>
-      <c r="D97">
-        <v>3</v>
-      </c>
-      <c r="E97">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A98">
-        <f t="shared" si="1"/>
-        <v>960</v>
-      </c>
-      <c r="B98" t="s">
-        <v>10</v>
-      </c>
-      <c r="C98" t="s">
-        <v>14</v>
-      </c>
-      <c r="D98">
-        <v>3</v>
-      </c>
-      <c r="E98">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A99">
-        <f t="shared" si="1"/>
-        <v>970</v>
-      </c>
-      <c r="B99" t="s">
-        <v>10</v>
-      </c>
-      <c r="C99" t="s">
-        <v>14</v>
-      </c>
-      <c r="D99">
-        <v>3</v>
-      </c>
-      <c r="E99">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A100">
-        <f t="shared" si="1"/>
-        <v>980</v>
-      </c>
-      <c r="B100" t="s">
-        <v>10</v>
-      </c>
-      <c r="C100" t="s">
-        <v>14</v>
-      </c>
-      <c r="D100">
-        <v>3</v>
-      </c>
-      <c r="E100">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A101">
-        <f t="shared" si="1"/>
-        <v>990</v>
-      </c>
-      <c r="B101" t="s">
-        <v>10</v>
-      </c>
-      <c r="C101" t="s">
-        <v>15</v>
-      </c>
-      <c r="D101">
-        <v>3</v>
-      </c>
-      <c r="E101">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A102">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="B102" t="s">
-        <v>10</v>
-      </c>
-      <c r="C102" t="s">
-        <v>15</v>
-      </c>
-      <c r="D102">
-        <v>3</v>
-      </c>
-      <c r="E102">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A103">
-        <f t="shared" si="1"/>
-        <v>1010</v>
-      </c>
-      <c r="B103" t="s">
-        <v>10</v>
-      </c>
-      <c r="C103" t="s">
-        <v>19</v>
       </c>
       <c r="D103">
         <v>3</v>
@@ -2331,16 +2338,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
         <f t="shared" si="1"/>
         <v>1020</v>
       </c>
       <c r="B104" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C104" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D104">
         <v>3</v>
@@ -2349,16 +2356,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
         <f t="shared" si="1"/>
         <v>1030</v>
       </c>
       <c r="B105" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C105" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D105">
         <v>3</v>
@@ -2367,16 +2374,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
         <f t="shared" si="1"/>
         <v>1040</v>
       </c>
       <c r="B106" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C106" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D106">
         <v>3</v>
@@ -2385,16 +2392,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
         <f t="shared" si="1"/>
         <v>1050</v>
       </c>
       <c r="B107" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C107" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D107">
         <v>3</v>
@@ -2403,16 +2410,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
         <f t="shared" si="1"/>
         <v>1060</v>
       </c>
       <c r="B108" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C108" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D108">
         <v>3</v>
@@ -2421,16 +2428,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
         <f t="shared" si="1"/>
         <v>1070</v>
       </c>
       <c r="B109" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C109" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D109">
         <v>3</v>
@@ -2439,16 +2446,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
         <f t="shared" si="1"/>
         <v>1080</v>
       </c>
       <c r="B110" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C110" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D110">
         <v>3</v>
@@ -2457,16 +2464,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
         <f t="shared" si="1"/>
         <v>1090</v>
       </c>
       <c r="B111" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C111" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D111">
         <v>3</v>
@@ -2475,16 +2482,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
         <f t="shared" si="1"/>
         <v>1100</v>
       </c>
       <c r="B112" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C112" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D112">
         <v>3</v>
@@ -2493,16 +2500,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
         <f t="shared" si="1"/>
         <v>1110</v>
       </c>
       <c r="B113" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C113" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D113">
         <v>3</v>
@@ -2511,16 +2518,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
         <f t="shared" si="1"/>
         <v>1120</v>
       </c>
       <c r="B114" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C114" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D114">
         <v>3</v>
@@ -2529,16 +2536,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
         <f t="shared" si="1"/>
         <v>1130</v>
       </c>
       <c r="B115" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C115" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D115">
         <v>3</v>
@@ -2547,16 +2554,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116">
         <f t="shared" si="1"/>
         <v>1140</v>
       </c>
       <c r="B116" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C116" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D116">
         <v>3</v>
@@ -2565,16 +2572,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117">
         <f t="shared" si="1"/>
         <v>1150</v>
       </c>
       <c r="B117" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C117" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D117">
         <v>3</v>
@@ -2583,16 +2590,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
         <f t="shared" si="1"/>
         <v>1160</v>
       </c>
       <c r="B118" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C118" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D118">
         <v>3</v>
@@ -2601,16 +2608,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119">
         <f t="shared" si="1"/>
         <v>1170</v>
       </c>
       <c r="B119" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C119" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D119">
         <v>3</v>
@@ -2619,16 +2626,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120">
         <f t="shared" si="1"/>
         <v>1180</v>
       </c>
       <c r="B120" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C120" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D120">
         <v>3</v>
@@ -2637,16 +2644,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121">
         <f t="shared" si="1"/>
         <v>1190</v>
       </c>
       <c r="B121" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C121" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D121">
         <v>3</v>
@@ -2655,16 +2662,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122">
         <f t="shared" si="1"/>
         <v>1200</v>
       </c>
       <c r="B122" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C122" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D122">
         <v>3</v>
@@ -2673,16 +2680,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123">
         <f t="shared" si="1"/>
         <v>1210</v>
       </c>
       <c r="B123" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C123" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D123">
         <v>3</v>
@@ -2691,16 +2698,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124">
         <f t="shared" si="1"/>
         <v>1220</v>
       </c>
       <c r="B124" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C124" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D124">
         <v>3</v>
@@ -2709,16 +2716,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125">
         <f t="shared" si="1"/>
         <v>1230</v>
       </c>
       <c r="B125" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C125" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D125">
         <v>3</v>
@@ -2727,16 +2734,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126">
         <f t="shared" si="1"/>
         <v>1240</v>
       </c>
       <c r="B126" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C126" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D126">
         <v>3</v>
@@ -2745,16 +2752,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127">
         <f t="shared" si="1"/>
         <v>1250</v>
       </c>
       <c r="B127" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C127" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D127">
         <v>4</v>
@@ -2763,16 +2770,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128">
         <f t="shared" si="1"/>
         <v>1260</v>
       </c>
       <c r="B128" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C128" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D128">
         <v>3</v>
@@ -2781,16 +2788,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129">
         <f t="shared" si="1"/>
         <v>1270</v>
       </c>
       <c r="B129" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C129" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D129">
         <v>3</v>
@@ -2799,16 +2806,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130">
         <f t="shared" si="1"/>
         <v>1280</v>
       </c>
       <c r="B130" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C130" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D130">
         <v>3</v>
@@ -2817,16 +2824,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131">
         <f t="shared" si="1"/>
         <v>1290</v>
       </c>
       <c r="B131" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C131" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D131">
         <v>3</v>
@@ -2835,16 +2842,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132">
         <f t="shared" si="1"/>
         <v>1300</v>
       </c>
       <c r="B132" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C132" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D132">
         <v>3</v>
@@ -2853,16 +2860,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133">
         <f t="shared" si="1"/>
         <v>1310</v>
       </c>
       <c r="B133" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C133" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D133">
         <v>3</v>
@@ -2871,16 +2878,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134">
         <f t="shared" si="1"/>
         <v>1320</v>
       </c>
       <c r="B134" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C134" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D134">
         <v>3</v>
@@ -2889,16 +2896,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135">
         <f t="shared" ref="A135:A198" si="2">A134 + 10</f>
         <v>1330</v>
       </c>
       <c r="B135" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C135" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D135">
         <v>3</v>
@@ -2907,16 +2914,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136">
         <f t="shared" si="2"/>
         <v>1340</v>
       </c>
       <c r="B136" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C136" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D136">
         <v>3</v>
@@ -2925,16 +2932,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137">
         <f t="shared" si="2"/>
         <v>1350</v>
       </c>
       <c r="B137" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C137" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D137">
         <v>3</v>
@@ -2943,16 +2950,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138">
         <f t="shared" si="2"/>
         <v>1360</v>
       </c>
       <c r="B138" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C138" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D138">
         <v>3</v>
@@ -2961,16 +2968,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139">
         <f t="shared" si="2"/>
         <v>1370</v>
       </c>
       <c r="B139" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C139" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D139">
         <v>3</v>
@@ -2979,16 +2986,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140">
         <f t="shared" si="2"/>
         <v>1380</v>
       </c>
       <c r="B140" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C140" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D140">
         <v>4</v>
@@ -2997,16 +3004,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141">
         <f t="shared" si="2"/>
         <v>1390</v>
       </c>
       <c r="B141" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C141" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D141">
         <v>3</v>
@@ -3015,16 +3022,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142">
         <f t="shared" si="2"/>
         <v>1400</v>
       </c>
       <c r="B142" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C142" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D142">
         <v>3</v>
@@ -3033,16 +3040,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143">
         <f t="shared" si="2"/>
         <v>1410</v>
       </c>
       <c r="B143" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C143" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D143">
         <v>3</v>
@@ -3051,16 +3058,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144">
         <f t="shared" si="2"/>
         <v>1420</v>
       </c>
       <c r="B144" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C144" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D144">
         <v>3</v>
@@ -3069,16 +3076,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145">
         <f t="shared" si="2"/>
         <v>1430</v>
       </c>
       <c r="B145" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C145" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D145">
         <v>3</v>
@@ -3087,16 +3094,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146">
         <f t="shared" si="2"/>
         <v>1440</v>
       </c>
       <c r="B146" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C146" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D146">
         <v>3</v>
@@ -3105,16 +3112,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147">
         <f t="shared" si="2"/>
         <v>1450</v>
       </c>
       <c r="B147" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C147" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D147">
         <v>3</v>
@@ -3123,16 +3130,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148">
         <f t="shared" si="2"/>
         <v>1460</v>
       </c>
       <c r="B148" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C148" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D148">
         <v>3</v>
@@ -3141,16 +3148,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149">
         <f t="shared" si="2"/>
         <v>1470</v>
       </c>
       <c r="B149" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C149" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D149">
         <v>3</v>
@@ -3159,16 +3166,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150">
         <f t="shared" si="2"/>
         <v>1480</v>
       </c>
       <c r="B150" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C150" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D150">
         <v>3</v>
@@ -3177,16 +3184,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151">
         <f t="shared" si="2"/>
         <v>1490</v>
       </c>
       <c r="B151" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C151" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D151">
         <v>3</v>
@@ -3195,16 +3202,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152">
         <f t="shared" si="2"/>
         <v>1500</v>
       </c>
       <c r="B152" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C152" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D152">
         <v>3</v>
@@ -3213,16 +3220,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153">
         <f t="shared" si="2"/>
         <v>1510</v>
       </c>
       <c r="B153" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C153" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D153">
         <v>3</v>
@@ -3231,16 +3238,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154">
         <f t="shared" si="2"/>
         <v>1520</v>
       </c>
       <c r="B154" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C154" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D154">
         <v>3</v>
@@ -3249,16 +3256,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155">
         <f t="shared" si="2"/>
         <v>1530</v>
       </c>
       <c r="B155" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C155" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D155">
         <v>3</v>
@@ -3267,16 +3274,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156">
         <f t="shared" si="2"/>
         <v>1540</v>
       </c>
       <c r="B156" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C156" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D156">
         <v>3</v>
@@ -3285,16 +3292,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157">
         <f t="shared" si="2"/>
         <v>1550</v>
       </c>
       <c r="B157" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C157" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D157">
         <v>3</v>
@@ -3303,16 +3310,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158">
         <f t="shared" si="2"/>
         <v>1560</v>
       </c>
       <c r="B158" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C158" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D158">
         <v>3</v>
@@ -3321,16 +3328,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159">
         <f t="shared" si="2"/>
         <v>1570</v>
       </c>
       <c r="B159" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C159" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D159">
         <v>4</v>
@@ -3339,16 +3346,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160">
         <f t="shared" si="2"/>
         <v>1580</v>
       </c>
       <c r="B160" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C160" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D160">
         <v>3</v>
@@ -3357,16 +3364,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161">
         <f t="shared" si="2"/>
         <v>1590</v>
       </c>
       <c r="B161" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C161" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D161">
         <v>3</v>
@@ -3375,16 +3382,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162">
         <f t="shared" si="2"/>
         <v>1600</v>
       </c>
       <c r="B162" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C162" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D162">
         <v>3</v>
@@ -3393,16 +3400,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163">
         <f t="shared" si="2"/>
         <v>1610</v>
       </c>
       <c r="B163" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C163" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D163">
         <v>3</v>
@@ -3411,16 +3418,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164">
         <f t="shared" si="2"/>
         <v>1620</v>
       </c>
       <c r="B164" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C164" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D164">
         <v>3</v>
@@ -3429,16 +3436,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165">
         <f t="shared" si="2"/>
         <v>1630</v>
       </c>
       <c r="B165" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C165" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D165">
         <v>3</v>
@@ -3447,16 +3454,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166">
         <f t="shared" si="2"/>
         <v>1640</v>
       </c>
       <c r="B166" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C166" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D166">
         <v>3</v>
@@ -3465,19 +3472,19 @@
         <v>3</v>
       </c>
       <c r="F166" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167">
         <f t="shared" si="2"/>
         <v>1650</v>
       </c>
       <c r="B167" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C167" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D167">
         <v>3</v>
@@ -3486,16 +3493,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168">
         <f t="shared" si="2"/>
         <v>1660</v>
       </c>
       <c r="B168" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C168" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D168">
         <v>3</v>
@@ -3504,16 +3511,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169">
         <f t="shared" si="2"/>
         <v>1670</v>
       </c>
       <c r="B169" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C169" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D169">
         <v>3</v>
@@ -3522,16 +3529,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170">
         <f t="shared" si="2"/>
         <v>1680</v>
       </c>
       <c r="B170" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C170" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D170">
         <v>4</v>
@@ -3540,16 +3547,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171">
         <f t="shared" si="2"/>
         <v>1690</v>
       </c>
       <c r="B171" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C171" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D171">
         <v>4</v>
@@ -3558,16 +3565,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172">
         <f t="shared" si="2"/>
         <v>1700</v>
       </c>
       <c r="B172" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C172" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D172">
         <v>4</v>
@@ -3576,16 +3583,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173">
         <f t="shared" si="2"/>
         <v>1710</v>
       </c>
       <c r="B173" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C173" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D173">
         <v>3</v>
@@ -3594,16 +3601,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174">
         <f t="shared" si="2"/>
         <v>1720</v>
       </c>
       <c r="B174" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C174" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D174">
         <v>3</v>
@@ -3612,16 +3619,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175">
         <f t="shared" si="2"/>
         <v>1730</v>
       </c>
       <c r="B175" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C175" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D175">
         <v>3</v>
@@ -3630,16 +3637,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176">
         <f t="shared" si="2"/>
         <v>1740</v>
       </c>
       <c r="B176" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C176" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D176">
         <v>3</v>
@@ -3648,16 +3655,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177">
         <f t="shared" si="2"/>
         <v>1750</v>
       </c>
       <c r="B177" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C177" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D177">
         <v>3</v>
@@ -3666,16 +3673,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178">
         <f t="shared" si="2"/>
         <v>1760</v>
       </c>
       <c r="B178" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C178" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D178">
         <v>3</v>
@@ -3684,16 +3691,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179">
         <f t="shared" si="2"/>
         <v>1770</v>
       </c>
       <c r="B179" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C179" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D179">
         <v>3</v>
@@ -3702,16 +3709,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180">
         <f t="shared" si="2"/>
         <v>1780</v>
       </c>
       <c r="B180" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C180" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D180">
         <v>4</v>
@@ -3720,16 +3727,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181">
         <f t="shared" si="2"/>
         <v>1790</v>
       </c>
       <c r="B181" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C181" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D181">
         <v>3</v>
@@ -3738,16 +3745,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182">
         <f t="shared" si="2"/>
         <v>1800</v>
       </c>
       <c r="B182" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C182" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D182">
         <v>4</v>
@@ -3756,16 +3763,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183">
         <f t="shared" si="2"/>
         <v>1810</v>
       </c>
       <c r="B183" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C183" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D183">
         <v>3</v>
@@ -3774,16 +3781,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184">
         <f t="shared" si="2"/>
         <v>1820</v>
       </c>
       <c r="B184" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C184" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D184">
         <v>3</v>
@@ -3792,16 +3799,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185">
         <f t="shared" si="2"/>
         <v>1830</v>
       </c>
       <c r="B185" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C185" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D185">
         <v>3</v>
@@ -3810,16 +3817,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186">
         <f t="shared" si="2"/>
         <v>1840</v>
       </c>
       <c r="B186" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C186" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D186">
         <v>3</v>
@@ -3828,16 +3835,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187">
         <f t="shared" si="2"/>
         <v>1850</v>
       </c>
       <c r="B187" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C187" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D187">
         <v>3</v>
@@ -3846,16 +3853,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188">
         <f t="shared" si="2"/>
         <v>1860</v>
       </c>
       <c r="B188" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C188" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D188">
         <v>3</v>
@@ -3864,16 +3871,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189">
         <f t="shared" si="2"/>
         <v>1870</v>
       </c>
       <c r="B189" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C189" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D189">
         <v>3</v>
@@ -3882,16 +3889,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190">
         <f t="shared" si="2"/>
         <v>1880</v>
       </c>
       <c r="B190" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C190" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D190">
         <v>3</v>
@@ -3900,16 +3907,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191">
         <f t="shared" si="2"/>
         <v>1890</v>
       </c>
       <c r="B191" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C191" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D191">
         <v>3</v>
@@ -3918,16 +3925,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192">
         <f t="shared" si="2"/>
         <v>1900</v>
       </c>
       <c r="B192" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C192" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D192">
         <v>3</v>
@@ -3936,16 +3943,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193">
         <f t="shared" si="2"/>
         <v>1910</v>
       </c>
       <c r="B193" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C193" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D193">
         <v>3</v>
@@ -3954,16 +3961,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194">
         <f t="shared" si="2"/>
         <v>1920</v>
       </c>
       <c r="B194" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C194" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D194">
         <v>3</v>
@@ -3972,16 +3979,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195">
         <f t="shared" si="2"/>
         <v>1930</v>
       </c>
       <c r="B195" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C195" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D195">
         <v>3</v>
@@ -3990,16 +3997,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196">
         <f t="shared" si="2"/>
         <v>1940</v>
       </c>
       <c r="B196" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C196" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D196">
         <v>4</v>
@@ -4008,16 +4015,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197">
         <f t="shared" si="2"/>
         <v>1950</v>
       </c>
       <c r="B197" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C197" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D197">
         <v>3</v>
@@ -4026,16 +4033,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198">
         <f t="shared" si="2"/>
         <v>1960</v>
       </c>
       <c r="B198" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C198" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D198">
         <v>3</v>
@@ -4044,16 +4051,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199">
-        <f t="shared" ref="A199:A262" si="3">A198 + 10</f>
+        <f t="shared" ref="A199:A219" si="3">A198 + 10</f>
         <v>1970</v>
       </c>
       <c r="B199" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C199" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D199">
         <v>3</v>
@@ -4062,16 +4069,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200">
         <f t="shared" si="3"/>
         <v>1980</v>
       </c>
       <c r="B200" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C200" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D200">
         <v>3</v>
@@ -4080,16 +4087,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201">
         <f t="shared" si="3"/>
         <v>1990</v>
       </c>
       <c r="B201" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C201" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D201">
         <v>3</v>
@@ -4098,16 +4105,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202">
         <f t="shared" si="3"/>
         <v>2000</v>
       </c>
       <c r="B202" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C202" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D202">
         <v>3</v>
@@ -4116,16 +4123,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203">
         <f t="shared" si="3"/>
         <v>2010</v>
       </c>
       <c r="B203" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C203" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D203">
         <v>3</v>
@@ -4134,16 +4141,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204">
         <f t="shared" si="3"/>
         <v>2020</v>
       </c>
       <c r="B204" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C204" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D204">
         <v>3</v>
@@ -4152,16 +4159,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205">
         <f t="shared" si="3"/>
         <v>2030</v>
       </c>
       <c r="B205" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C205" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D205">
         <v>3</v>
@@ -4170,16 +4177,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206">
         <f t="shared" si="3"/>
         <v>2040</v>
       </c>
       <c r="B206" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C206" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D206">
         <v>3</v>
@@ -4188,16 +4195,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207">
         <f t="shared" si="3"/>
         <v>2050</v>
       </c>
       <c r="B207" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C207" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D207">
         <v>3</v>
@@ -4206,16 +4213,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208">
         <f t="shared" si="3"/>
         <v>2060</v>
       </c>
       <c r="B208" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C208" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D208">
         <v>3</v>
@@ -4224,16 +4231,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209">
         <f t="shared" si="3"/>
         <v>2070</v>
       </c>
       <c r="B209" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C209" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D209">
         <v>3</v>
@@ -4242,16 +4249,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210">
         <f t="shared" si="3"/>
         <v>2080</v>
       </c>
       <c r="B210" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C210" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D210">
         <v>3</v>
@@ -4260,16 +4267,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211">
         <f t="shared" si="3"/>
         <v>2090</v>
       </c>
       <c r="B211" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C211" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D211">
         <v>3</v>
@@ -4278,16 +4285,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212">
         <f t="shared" si="3"/>
         <v>2100</v>
       </c>
       <c r="B212" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C212" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D212">
         <v>3</v>
@@ -4296,16 +4303,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213">
         <f t="shared" si="3"/>
         <v>2110</v>
       </c>
       <c r="B213" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C213" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D213">
         <v>3</v>
@@ -4314,16 +4321,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214">
         <f t="shared" si="3"/>
         <v>2120</v>
       </c>
       <c r="B214" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C214" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D214">
         <v>3</v>
@@ -4332,16 +4339,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215">
         <f t="shared" si="3"/>
         <v>2130</v>
       </c>
       <c r="B215" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C215" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D215">
         <v>3</v>
@@ -4350,16 +4357,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216">
         <f t="shared" si="3"/>
         <v>2140</v>
       </c>
       <c r="B216" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C216" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D216">
         <v>3</v>
@@ -4368,16 +4375,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217">
         <f t="shared" si="3"/>
         <v>2150</v>
       </c>
       <c r="B217" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C217" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D217">
         <v>3</v>
@@ -4386,16 +4393,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218">
         <f t="shared" si="3"/>
         <v>2160</v>
       </c>
       <c r="B218" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C218" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D218">
         <v>3</v>
@@ -4404,16 +4411,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219">
         <f t="shared" si="3"/>
         <v>2170</v>
       </c>
       <c r="B219" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C219" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D219">
         <v>3</v>
@@ -4422,7 +4429,7 @@
         <v>3</v>
       </c>
       <c r="F219" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>